<commit_message>
update to the fitted NRP1 excel sheet data
</commit_message>
<xml_diff>
--- a/data/VEGFA165_VEGFR2_NRP1_fitted_binding_kinetics.xlsx
+++ b/data/VEGFA165_VEGFR2_NRP1_fitted_binding_kinetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18ADAEE-B4A8-4AE2-8E41-09554A347E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE2699-2B03-415A-B515-4D91A887A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
       </c>
       <c r="G3" s="2">
         <f>Sheet2!H7</f>
-        <v>21669633.776685923</v>
+        <v>23294878.560656402</v>
       </c>
       <c r="H3" s="2">
         <v>8.0490000000000006E-3</v>
@@ -594,7 +594,7 @@
       </c>
       <c r="K3" s="2">
         <f>STDEV(Sheet2!K7:K11)/SQRT(5)</f>
-        <v>5.7803050891635056E-11</v>
+        <v>5.8905524473255032E-11</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -739,7 +739,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,11 +1002,11 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="2">
-        <v>119397500</v>
+        <v>128404400</v>
       </c>
       <c r="H7" s="7">
         <f>STDEV(G7:G11)/SQRT(5)</f>
-        <v>21669633.776685923</v>
+        <v>23294878.560656402</v>
       </c>
       <c r="I7" s="2">
         <v>1.7746000000000001E-2</v>
@@ -1017,11 +1017,11 @@
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
-        <v>1.4862957767122428E-10</v>
+        <v>1.3820398677926926E-10</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" ref="L7" si="2">STDEV(K7:K11)/SQRT(5)</f>
-        <v>5.7803050891635056E-11</v>
+        <v>5.8905524473255032E-11</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>87856320</v>
+        <v>91080760</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="2">
@@ -1057,7 +1057,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>1.0691319645530339E-10</v>
+        <v>1.0312825672513054E-10</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="2"/>
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="2">
-        <v>32306270</v>
+        <v>32735990</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="2">
@@ -1094,7 +1094,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="2">
         <f t="shared" si="0"/>
-        <v>1.7380527061774697E-10</v>
+        <v>1.7152375718589846E-10</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="2"/>
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="2">
-        <v>18378530</v>
+        <v>18411490</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="2">
@@ -1131,7 +1131,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="2">
         <f t="shared" si="0"/>
-        <v>2.4844206799999783E-10</v>
+        <v>2.479973103752059E-10</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="2"/>
@@ -1159,7 +1159,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="4">
-        <v>6728897</v>
+        <v>6732888</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="4">
@@ -1168,7 +1168,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>4.3454372982674573E-10</v>
+        <v>4.3428614882647682E-10</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="2"/>

</xml_diff>

<commit_message>
update kd of NRP1 fitted data excel sheet
</commit_message>
<xml_diff>
--- a/data/VEGFA165_VEGFR2_NRP1_fitted_binding_kinetics.xlsx
+++ b/data/VEGFA165_VEGFR2_NRP1_fitted_binding_kinetics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE2699-2B03-415A-B515-4D91A887A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E16F718-BE48-4D4D-92DF-56C5FE65F0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,8 +468,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,8 +546,8 @@
         <v>8.5380507143024184E-4</v>
       </c>
       <c r="J2" s="2">
-        <f>H2/F2</f>
-        <v>1.6940998975549024E-9</v>
+        <f>AVERAGE(Sheet2!I2:I6)/AVERAGE(Sheet2!G2:G6)</f>
+        <v>1.6941075330403121E-9</v>
       </c>
       <c r="K2" s="2">
         <f>STDEV(Sheet2!K2:K6)/SQRT(5)</f>
@@ -589,8 +589,8 @@
         <v>2.6472572107749544E-3</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J4" si="0">H3/F3</f>
-        <v>1.4509732733571276E-10</v>
+        <f>AVERAGE(Sheet2!I7:I11)/AVERAGE(Sheet2!G7:G11)</f>
+        <v>1.4509373349380319E-10</v>
       </c>
       <c r="K3" s="2">
         <f>STDEV(Sheet2!K7:K11)/SQRT(5)</f>
@@ -622,7 +622,7 @@
       </c>
       <c r="G4" s="2">
         <f>Sheet2!H12</f>
-        <v>14059388.174998786</v>
+        <v>14362286.542042786</v>
       </c>
       <c r="H4" s="2">
         <v>4.1279999999999997E-3</v>
@@ -632,12 +632,12 @@
         <v>2.8144278281739605E-4</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1541190699723826E-10</v>
+        <f>AVERAGE(Sheet2!I12:I16)/AVERAGE(Sheet2!G12:G16)</f>
+        <v>1.1540632953196808E-10</v>
       </c>
       <c r="K4" s="2">
         <f>STDEV(Sheet2!K12:K16)/SQRT(5)</f>
-        <v>7.3324162206172232E-11</v>
+        <v>7.3439181551013084E-11</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -738,8 +738,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,11 +1196,11 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="2">
-        <v>85442310</v>
+        <v>87144780</v>
       </c>
       <c r="H12" s="7">
         <f t="shared" ref="H12" si="3">STDEV(G12:G16)/SQRT(5)</f>
-        <v>14059388.174998786</v>
+        <v>14362286.542042786</v>
       </c>
       <c r="I12" s="2">
         <v>4.9740000000000001E-3</v>
@@ -1211,11 +1211,11 @@
       </c>
       <c r="K12" s="2">
         <f t="shared" si="0"/>
-        <v>5.8214718211621385E-11</v>
+        <v>5.707742907836821E-11</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" ref="L12" si="5">STDEV(K12:K16)/SQRT(5)</f>
-        <v>7.3324162206172232E-11</v>
+        <v>7.3439181551013084E-11</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2">
-        <v>45213570</v>
+        <v>45296290</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="2">
@@ -1251,7 +1251,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="2">
         <f t="shared" si="0"/>
-        <v>1.0010269040909621E-10</v>
+        <v>9.9919883063270741E-11</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="2"/>
@@ -1279,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="2">
-        <v>24827940</v>
+        <v>24892240</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="2">
@@ -1288,7 +1288,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="2">
         <f t="shared" si="0"/>
-        <v>1.565172140741439E-10</v>
+        <v>1.5611290908331271E-10</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="2"/>
@@ -1316,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="2">
-        <v>14292990</v>
+        <v>14307420</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="2">
@@ -1325,7 +1325,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>2.7279106750931751E-10</v>
+        <v>2.7251593928185515E-10</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="2"/>
@@ -1353,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="2">
-        <v>7195128</v>
+        <v>7196948</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="2">
@@ -1362,7 +1362,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="2">
         <f t="shared" si="0"/>
-        <v>4.6614876066138089E-10</v>
+        <v>4.6603087864466993E-10</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="2"/>

</xml_diff>